<commit_message>
Updated with pAUC and CIs
</commit_message>
<xml_diff>
--- a/data/tutorial/test1_fitparams.xlsx
+++ b/data/tutorial/test1_fitparams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10106"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10203"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sboogert/Dropbox (Royal Holloway)/Psychology/pyWitness/data/tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AC6C12-6FA3-6C47-A0C9-7C060E0C995E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0330EC2E-21B3-AD49-A46E-D0042C13E360}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="2760" windowWidth="29680" windowHeight="16940" xr2:uid="{7A0DD3CD-3870-5644-AD65-7D6B63D4FA1A}"/>
+    <workbookView xWindow="45900" yWindow="1400" windowWidth="36820" windowHeight="16940" xr2:uid="{7A0DD3CD-3870-5644-AD65-7D6B63D4FA1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>lureMean</t>
   </si>
@@ -80,12 +80,24 @@
   </si>
   <si>
     <t>BEST-REST</t>
+  </si>
+  <si>
+    <t>pAUC</t>
+  </si>
+  <si>
+    <t>pAUC lower 95% CL</t>
+  </si>
+  <si>
+    <t>pAUC upper 95% CL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -123,15 +135,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -448,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83572180-BEB5-D240-8CE3-CD6E04FC80F2}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,244 +480,268 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
         <v>0</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
         <v>1</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>1.7478107994751699</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>1.66438995763123</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>1.7983028256957301</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>1.79842922628878</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="4">
         <v>2.1515418771457</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
         <v>1</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
         <v>0.47639080106294002</v>
       </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
         <v>-3.2773907055522597E-5</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
         <v>0.47639080106294002</v>
       </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
         <v>-3.2773907055522597E-5</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>1.7478107994751699</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>1.3609961250836899</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>1.3482358266805601</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>1.6178836879724401</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
         <v>0.82021777142498598</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="4">
         <v>1.9613365467695101</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>1.8627149509844101</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>1.71830343944034</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>2.0819197901106299</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="4">
         <v>2.3724731528667302</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="4">
         <v>2.6279666081478901</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>2.56594923309612</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>2.3078475100741902</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>2.76937383377388</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="4">
         <v>4.3883441517683996</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="4">
         <v>17.060787052372302</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <v>13.485689914476101</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>29.997916048259899</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <v>29.9979143219152</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="4">
         <v>20.195630845996</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2.1746073272763299E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.87126054720755E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2.4982594572062901E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>